<commit_message>
feat: Use excel date format
</commit_message>
<xml_diff>
--- a/assets/template.xlsx
+++ b/assets/template.xlsx
@@ -28,7 +28,7 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing">
   <authors>
-    <author>Unknown Author</author>
+    <author>Unbekannter Autor</author>
   </authors>
   <commentList>
     <comment ref="A1" authorId="0">
@@ -51,7 +51,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Format: JJJJ-MM-TT HH:MM:SS</t>
+          <t xml:space="preserve">Spalte im Dattumsformat mit Stunde und Minute</t>
         </r>
       </text>
     </comment>
@@ -63,7 +63,7 @@
             <rFont val="Arial"/>
             <family val="2"/>
           </rPr>
-          <t xml:space="preserve">Format: JJJJ-MM-TT HH:MM:SS</t>
+          <t xml:space="preserve">Spalte im Dattumsformat mit Stunde und Minute</t>
         </r>
       </text>
     </comment>
@@ -239,24 +239,28 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -452,434 +456,434 @@
   <dimension ref="A1:G50"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G10" activeCellId="0" sqref="G10"/>
+      <selection pane="topLeft" activeCell="C1" activeCellId="0" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.6796875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="39.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="20.07"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="6.19"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="7.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="14.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="18.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="39.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="22.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="20.07"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="6.19"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="7.11"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="14.39"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="18.16"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="E1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="F1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="G1" s="2" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B2" s="2"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4"/>
-      <c r="F2" s="4"/>
-      <c r="G2" s="4"/>
+      <c r="B2" s="3"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B3" s="2"/>
-      <c r="C3" s="3"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
+      <c r="B3" s="3"/>
+      <c r="C3" s="4"/>
+      <c r="D3" s="5"/>
+      <c r="E3" s="5"/>
+      <c r="F3" s="5"/>
+      <c r="G3" s="5"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B4" s="2"/>
-      <c r="C4" s="3"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
+      <c r="B4" s="3"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B5" s="2"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+      <c r="G5" s="5"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B6" s="2"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B7" s="2"/>
-      <c r="C7" s="3"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="4"/>
-      <c r="G7" s="4"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B8" s="2"/>
-      <c r="C8" s="3"/>
-      <c r="D8" s="4"/>
-      <c r="E8" s="4"/>
-      <c r="F8" s="4"/>
-      <c r="G8" s="4"/>
+      <c r="B8" s="3"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B9" s="2"/>
-      <c r="C9" s="3"/>
-      <c r="D9" s="4"/>
-      <c r="E9" s="4"/>
-      <c r="F9" s="4"/>
-      <c r="G9" s="4"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="4"/>
+      <c r="D9" s="5"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="5"/>
+      <c r="G9" s="5"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B10" s="2"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="4"/>
-      <c r="E10" s="4"/>
-      <c r="F10" s="4"/>
-      <c r="G10" s="4"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B11" s="2"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="4"/>
-      <c r="E11" s="4"/>
-      <c r="F11" s="4"/>
-      <c r="G11" s="4"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="5"/>
+      <c r="E11" s="5"/>
+      <c r="F11" s="5"/>
+      <c r="G11" s="5"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B12" s="2"/>
-      <c r="C12" s="3"/>
-      <c r="D12" s="4"/>
-      <c r="E12" s="4"/>
-      <c r="F12" s="4"/>
-      <c r="G12" s="4"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B13" s="2"/>
-      <c r="C13" s="3"/>
-      <c r="D13" s="4"/>
-      <c r="E13" s="4"/>
-      <c r="F13" s="4"/>
-      <c r="G13" s="4"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="4"/>
+      <c r="D13" s="5"/>
+      <c r="E13" s="5"/>
+      <c r="F13" s="5"/>
+      <c r="G13" s="5"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B14" s="2"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="4"/>
-      <c r="E14" s="4"/>
-      <c r="F14" s="4"/>
-      <c r="G14" s="4"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B15" s="2"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="4"/>
-      <c r="E15" s="4"/>
-      <c r="F15" s="4"/>
-      <c r="G15" s="4"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="4"/>
+      <c r="D15" s="5"/>
+      <c r="E15" s="5"/>
+      <c r="F15" s="5"/>
+      <c r="G15" s="5"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B16" s="2"/>
-      <c r="C16" s="3"/>
-      <c r="D16" s="4"/>
-      <c r="E16" s="4"/>
-      <c r="F16" s="4"/>
-      <c r="G16" s="4"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B17" s="2"/>
-      <c r="C17" s="3"/>
-      <c r="D17" s="4"/>
-      <c r="E17" s="4"/>
-      <c r="F17" s="4"/>
-      <c r="G17" s="4"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="4"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B18" s="2"/>
-      <c r="C18" s="3"/>
-      <c r="D18" s="4"/>
-      <c r="E18" s="4"/>
-      <c r="F18" s="4"/>
-      <c r="G18" s="4"/>
+      <c r="B18" s="3"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B19" s="2"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="4"/>
-      <c r="E19" s="4"/>
-      <c r="F19" s="4"/>
-      <c r="G19" s="4"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="4"/>
+      <c r="D19" s="5"/>
+      <c r="E19" s="5"/>
+      <c r="F19" s="5"/>
+      <c r="G19" s="5"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B20" s="2"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="4"/>
-      <c r="E20" s="4"/>
-      <c r="F20" s="4"/>
-      <c r="G20" s="4"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B21" s="2"/>
-      <c r="C21" s="3"/>
-      <c r="D21" s="4"/>
-      <c r="E21" s="4"/>
-      <c r="F21" s="4"/>
-      <c r="G21" s="4"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="4"/>
+      <c r="D21" s="5"/>
+      <c r="E21" s="5"/>
+      <c r="F21" s="5"/>
+      <c r="G21" s="5"/>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B22" s="2"/>
-      <c r="C22" s="3"/>
-      <c r="D22" s="4"/>
-      <c r="E22" s="4"/>
-      <c r="F22" s="4"/>
-      <c r="G22" s="4"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B23" s="2"/>
-      <c r="C23" s="3"/>
-      <c r="D23" s="4"/>
-      <c r="E23" s="4"/>
-      <c r="F23" s="4"/>
-      <c r="G23" s="4"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="4"/>
+      <c r="D23" s="5"/>
+      <c r="E23" s="5"/>
+      <c r="F23" s="5"/>
+      <c r="G23" s="5"/>
     </row>
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B24" s="2"/>
-      <c r="C24" s="3"/>
-      <c r="D24" s="4"/>
-      <c r="E24" s="4"/>
-      <c r="F24" s="4"/>
-      <c r="G24" s="4"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B25" s="2"/>
-      <c r="C25" s="3"/>
-      <c r="D25" s="4"/>
-      <c r="E25" s="4"/>
-      <c r="F25" s="4"/>
-      <c r="G25" s="4"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="4"/>
+      <c r="D25" s="5"/>
+      <c r="E25" s="5"/>
+      <c r="F25" s="5"/>
+      <c r="G25" s="5"/>
     </row>
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B26" s="2"/>
-      <c r="C26" s="3"/>
-      <c r="D26" s="4"/>
-      <c r="E26" s="4"/>
-      <c r="F26" s="4"/>
-      <c r="G26" s="4"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B27" s="2"/>
-      <c r="C27" s="3"/>
-      <c r="D27" s="4"/>
-      <c r="E27" s="4"/>
-      <c r="F27" s="4"/>
-      <c r="G27" s="4"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="4"/>
+      <c r="D27" s="5"/>
+      <c r="E27" s="5"/>
+      <c r="F27" s="5"/>
+      <c r="G27" s="5"/>
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B28" s="2"/>
-      <c r="C28" s="3"/>
-      <c r="D28" s="4"/>
-      <c r="E28" s="4"/>
-      <c r="F28" s="4"/>
-      <c r="G28" s="4"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B29" s="2"/>
-      <c r="C29" s="3"/>
-      <c r="D29" s="4"/>
-      <c r="E29" s="4"/>
-      <c r="F29" s="4"/>
-      <c r="G29" s="4"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="4"/>
+      <c r="D29" s="5"/>
+      <c r="E29" s="5"/>
+      <c r="F29" s="5"/>
+      <c r="G29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B30" s="2"/>
-      <c r="C30" s="3"/>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4"/>
-      <c r="F30" s="4"/>
-      <c r="G30" s="4"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B31" s="2"/>
-      <c r="C31" s="3"/>
-      <c r="D31" s="4"/>
-      <c r="E31" s="4"/>
-      <c r="F31" s="4"/>
-      <c r="G31" s="4"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="4"/>
+      <c r="D31" s="5"/>
+      <c r="E31" s="5"/>
+      <c r="F31" s="5"/>
+      <c r="G31" s="5"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B32" s="2"/>
-      <c r="C32" s="3"/>
-      <c r="D32" s="4"/>
-      <c r="E32" s="4"/>
-      <c r="F32" s="4"/>
-      <c r="G32" s="4"/>
+      <c r="B32" s="3"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B33" s="2"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="4"/>
-      <c r="E33" s="4"/>
-      <c r="F33" s="4"/>
-      <c r="G33" s="4"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="4"/>
+      <c r="D33" s="5"/>
+      <c r="E33" s="5"/>
+      <c r="F33" s="5"/>
+      <c r="G33" s="5"/>
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B34" s="2"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="4"/>
-      <c r="E34" s="4"/>
-      <c r="F34" s="4"/>
-      <c r="G34" s="4"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="4"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B35" s="2"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="4"/>
-      <c r="E35" s="4"/>
-      <c r="F35" s="4"/>
-      <c r="G35" s="4"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="4"/>
+      <c r="D35" s="5"/>
+      <c r="E35" s="5"/>
+      <c r="F35" s="5"/>
+      <c r="G35" s="5"/>
     </row>
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B36" s="2"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="4"/>
-      <c r="E36" s="4"/>
-      <c r="F36" s="4"/>
-      <c r="G36" s="4"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="4"/>
+      <c r="D36" s="5"/>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5"/>
+      <c r="G36" s="5"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B37" s="2"/>
-      <c r="C37" s="3"/>
-      <c r="D37" s="4"/>
-      <c r="E37" s="4"/>
-      <c r="F37" s="4"/>
-      <c r="G37" s="4"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="4"/>
+      <c r="D37" s="5"/>
+      <c r="E37" s="5"/>
+      <c r="F37" s="5"/>
+      <c r="G37" s="5"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B38" s="2"/>
-      <c r="C38" s="3"/>
-      <c r="D38" s="4"/>
-      <c r="E38" s="4"/>
-      <c r="F38" s="4"/>
-      <c r="G38" s="4"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="4"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B39" s="2"/>
-      <c r="C39" s="3"/>
-      <c r="D39" s="4"/>
-      <c r="E39" s="4"/>
-      <c r="F39" s="4"/>
-      <c r="G39" s="4"/>
+      <c r="B39" s="3"/>
+      <c r="C39" s="4"/>
+      <c r="D39" s="5"/>
+      <c r="E39" s="5"/>
+      <c r="F39" s="5"/>
+      <c r="G39" s="5"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B40" s="2"/>
-      <c r="C40" s="3"/>
-      <c r="D40" s="4"/>
-      <c r="E40" s="4"/>
-      <c r="F40" s="4"/>
-      <c r="G40" s="4"/>
+      <c r="B40" s="3"/>
+      <c r="C40" s="4"/>
+      <c r="D40" s="5"/>
+      <c r="E40" s="5"/>
+      <c r="F40" s="5"/>
+      <c r="G40" s="5"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B41" s="2"/>
-      <c r="C41" s="3"/>
-      <c r="D41" s="4"/>
-      <c r="E41" s="4"/>
-      <c r="F41" s="4"/>
-      <c r="G41" s="4"/>
+      <c r="B41" s="3"/>
+      <c r="C41" s="4"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B42" s="2"/>
-      <c r="C42" s="3"/>
-      <c r="D42" s="4"/>
-      <c r="E42" s="4"/>
-      <c r="F42" s="4"/>
-      <c r="G42" s="4"/>
+      <c r="B42" s="3"/>
+      <c r="C42" s="4"/>
+      <c r="D42" s="5"/>
+      <c r="E42" s="5"/>
+      <c r="F42" s="5"/>
+      <c r="G42" s="5"/>
     </row>
     <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B43" s="2"/>
-      <c r="C43" s="3"/>
-      <c r="D43" s="4"/>
-      <c r="E43" s="4"/>
-      <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
+      <c r="B43" s="3"/>
+      <c r="C43" s="4"/>
+      <c r="D43" s="5"/>
+      <c r="E43" s="5"/>
+      <c r="F43" s="5"/>
+      <c r="G43" s="5"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B44" s="2"/>
-      <c r="C44" s="3"/>
-      <c r="D44" s="4"/>
-      <c r="E44" s="4"/>
-      <c r="F44" s="4"/>
-      <c r="G44" s="4"/>
+      <c r="B44" s="3"/>
+      <c r="C44" s="4"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B45" s="2"/>
-      <c r="C45" s="3"/>
-      <c r="D45" s="4"/>
-      <c r="E45" s="4"/>
-      <c r="F45" s="4"/>
-      <c r="G45" s="4"/>
+      <c r="B45" s="3"/>
+      <c r="C45" s="4"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
     </row>
     <row r="46" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B46" s="2"/>
-      <c r="C46" s="3"/>
-      <c r="D46" s="4"/>
-      <c r="E46" s="4"/>
-      <c r="F46" s="4"/>
-      <c r="G46" s="4"/>
+      <c r="B46" s="3"/>
+      <c r="C46" s="4"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
     </row>
     <row r="47" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B47" s="2"/>
-      <c r="C47" s="3"/>
-      <c r="D47" s="4"/>
-      <c r="E47" s="4"/>
-      <c r="F47" s="4"/>
-      <c r="G47" s="4"/>
+      <c r="B47" s="3"/>
+      <c r="C47" s="4"/>
+      <c r="D47" s="5"/>
+      <c r="E47" s="5"/>
+      <c r="F47" s="5"/>
+      <c r="G47" s="5"/>
     </row>
     <row r="48" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B48" s="2"/>
-      <c r="C48" s="3"/>
-      <c r="D48" s="4"/>
-      <c r="E48" s="4"/>
-      <c r="F48" s="4"/>
-      <c r="G48" s="4"/>
+      <c r="B48" s="3"/>
+      <c r="C48" s="4"/>
+      <c r="D48" s="5"/>
+      <c r="E48" s="5"/>
+      <c r="F48" s="5"/>
+      <c r="G48" s="5"/>
     </row>
     <row r="49" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B49" s="2"/>
-      <c r="C49" s="3"/>
-      <c r="D49" s="4"/>
-      <c r="E49" s="4"/>
-      <c r="F49" s="4"/>
-      <c r="G49" s="4"/>
+      <c r="B49" s="3"/>
+      <c r="C49" s="4"/>
+      <c r="D49" s="5"/>
+      <c r="E49" s="5"/>
+      <c r="F49" s="5"/>
+      <c r="G49" s="5"/>
     </row>
     <row r="50" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="B50" s="2"/>
-      <c r="C50" s="3"/>
-      <c r="D50" s="4"/>
-      <c r="E50" s="4"/>
-      <c r="F50" s="4"/>
-      <c r="G50" s="4"/>
+      <c r="B50" s="3"/>
+      <c r="C50" s="4"/>
+      <c r="D50" s="5"/>
+      <c r="E50" s="5"/>
+      <c r="F50" s="5"/>
+      <c r="G50" s="5"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>

</xml_diff>